<commit_message>
regex and form redesign
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aclem\Desktop\js\store-ref converter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albertclemente/Desktop/store-ref converter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFF9EE4-AB8A-432A-92FB-230AEC238DF6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA98055F-7A28-614D-AF58-3914C1253AFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CA5F7FEA-9875-4CA4-A99C-D49AC768C903}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{CA5F7FEA-9875-4CA4-A99C-D49AC768C903}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>store_ref</t>
   </si>
@@ -78,6 +78,21 @@
   </si>
   <si>
     <t>asdas&lt;&gt;@assada.com</t>
+  </si>
+  <si>
+    <t>K304-kjasjkasjjsa</t>
+  </si>
+  <si>
+    <t>adsassadas</t>
+  </si>
+  <si>
+    <t>(0034) 934561245</t>
+  </si>
+  <si>
+    <t>.-albert.clemente@test.com</t>
+  </si>
+  <si>
+    <t>0034934561245</t>
   </si>
 </sst>
 </file>
@@ -125,10 +140,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -444,20 +460,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27DAA58E-1703-45D8-A8E0-F9EC760AD4BD}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +487,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -485,7 +501,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -499,7 +515,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -513,7 +529,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>308</v>
       </c>
@@ -527,7 +543,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>308</v>
       </c>
@@ -539,6 +555,34 @@
       </c>
       <c r="D6" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -546,8 +590,10 @@
     <hyperlink ref="D2" r:id="rId1" xr:uid="{D7B71BE9-1882-43C5-B313-FB88BBFDAA21}"/>
     <hyperlink ref="D5" r:id="rId2" xr:uid="{7B079C47-E025-47E6-8FD8-94D707847A30}"/>
     <hyperlink ref="D6" r:id="rId3" display="asdas@assada.com" xr:uid="{9427D9F1-EEF0-4BCB-8D94-A7CA1F8DA151}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{6920844C-2DBE-3F47-B740-CDFD32B93403}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{D690A149-BC09-C740-BDA2-5B3DD0296A39}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>